<commit_message>
Updated TLRatio excel Biomass calculations, boxplot and PCO Notes cleaned
</commit_message>
<xml_diff>
--- a/Data/TLRatio.xlsx
+++ b/Data/TLRatio.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ejer\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ejer\Desktop\Github_UVC_DOVS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11FF25D-57E8-46E7-BD87-B740392F3285}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D1085F-843E-4D09-85FB-158392249179}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5C502FD-42F0-47CE-822F-E8D933141968}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t>SpeciesName</t>
   </si>
@@ -150,6 +150,21 @@
   </si>
   <si>
     <t>TLRatio</t>
+  </si>
+  <si>
+    <t>Caranx lugubris</t>
+  </si>
+  <si>
+    <t>Canthidermis maculata</t>
+  </si>
+  <si>
+    <t>Carcharhinus falciformis</t>
+  </si>
+  <si>
+    <t>Thunnus albacares</t>
+  </si>
+  <si>
+    <t>Euthynnus lineatus</t>
   </si>
 </sst>
 </file>
@@ -157,7 +172,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -191,7 +206,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1D2B53-9EAC-4FD1-858C-E31F7022FE8B}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,9 +535,12 @@
     <col min="4" max="4" width="9.44140625" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +560,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -562,7 +580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -582,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -602,7 +620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -622,7 +640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -642,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -662,7 +680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -682,7 +700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -702,7 +720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -722,7 +740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -739,11 +757,10 @@
         <v>11</v>
       </c>
       <c r="F11" s="2">
-        <f>1/1.043</f>
-        <v>0.95877277085330781</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.95877000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -760,11 +777,11 @@
         <v>8</v>
       </c>
       <c r="F12" s="2">
-        <f>1/((1.012+1.019+1.044)/3)</f>
-        <v>0.97560975609756106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.97560999999999998</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -781,11 +798,11 @@
         <v>8</v>
       </c>
       <c r="F13" s="2">
-        <f>((0.775+0.776)/2)</f>
-        <v>0.77550000000000008</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.77549999999999997</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -802,11 +819,11 @@
         <v>8</v>
       </c>
       <c r="F14" s="2">
-        <f>1/((1.052+1.084)/2)</f>
-        <v>0.93632958801498123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.93633</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -823,11 +840,11 @@
         <v>8</v>
       </c>
       <c r="F15" s="2">
-        <f>1/1.107</f>
-        <v>0.90334236675700097</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.90334000000000003</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -844,11 +861,11 @@
         <v>8</v>
       </c>
       <c r="F16" s="2">
-        <f>1/1.216</f>
-        <v>0.82236842105263164</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.82237000000000005</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -865,11 +882,11 @@
         <v>8</v>
       </c>
       <c r="F17" s="2">
-        <f>1/((1.109+1.162)/2)</f>
-        <v>0.8806693086745927</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.88066999999999995</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -889,7 +906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -909,7 +926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -929,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -949,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -969,7 +986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -989,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1006,6 +1023,107 @@
         <v>15</v>
       </c>
       <c r="F24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25">
+        <v>2.5100000000000001E-2</v>
+      </c>
+      <c r="D25">
+        <v>2.84</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25">
+        <v>0.86299999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="D26">
+        <v>3.0550000000000002</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27">
+        <v>4.6399999999999997E-2</v>
+      </c>
+      <c r="D27">
+        <v>2.75</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27">
+        <v>0.81721999999999995</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="D28">
+        <v>2.9809999999999999</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29">
+        <v>0.01</v>
+      </c>
+      <c r="D29">
+        <v>3.05</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29">
         <v>1</v>
       </c>
     </row>

</xml_diff>